<commit_message>
Change to pass signed weight directly
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/LnLikeLogisticTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/LnLikeLogisticTest.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace-STS\maven.1536042399911\jacobi\src\test\resources\jacobi\test\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24435" windowHeight="8685" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15615" windowHeight="7215"/>
   </bookViews>
   <sheets>
     <sheet name="test 3 vars with noise" sheetId="1" r:id="rId1"/>
@@ -17,6 +12,7 @@
     <sheet name="rand" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <oleSize ref="A1:N26"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -431,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L158"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119:A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -524,7 +520,7 @@
         <v>-7.8736879835035911E-2</v>
       </c>
       <c r="F8">
-        <f>IF(D8+E8&gt;0.5, 1, 0)</f>
+        <f>IF(D8+E8&gt;0.5, 1, -1)</f>
         <v>1</v>
       </c>
       <c r="G8">
@@ -2956,13 +2952,13 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119">
-        <f>F8</f>
+        <f>IF(F8 &gt; 0, 1, -1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120">
-        <f t="shared" ref="A120:A138" si="59">F9</f>
+        <f t="shared" ref="A120:A138" si="59">IF(F9 &gt; 0, 1, -1)</f>
         <v>1</v>
       </c>
     </row>
@@ -2975,7 +2971,7 @@
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -2993,7 +2989,7 @@
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -3005,7 +3001,7 @@
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
@@ -3023,7 +3019,7 @@
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
@@ -3040,8 +3036,8 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133">
-        <f>F22</f>
-        <v>0</v>
+        <f t="shared" si="59"/>
+        <v>-1</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
@@ -3053,7 +3049,7 @@
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
@@ -3065,7 +3061,7 @@
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
@@ -3225,8 +3221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3472,47 +3468,47 @@
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1">
         <f ca="1">2*RAND()-1</f>
-        <v>0.45759308825688549</v>
+        <v>-0.10502247738798531</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:K16" ca="1" si="0">2*RAND()-1</f>
-        <v>0.69580540479850028</v>
+        <v>-0.77349274052174799</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.50453484880388122</v>
+        <v>0.18012789077589386</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.94368821237050415</v>
+        <v>1.3943828785534684E-2</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.90815244238591775</v>
+        <v>-0.4378798137025286</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57181282656211319</v>
+        <v>-0.27545373525073891</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.9482091839327631</v>
+        <v>-0.16218503113544247</v>
       </c>
       <c r="H1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72019926673355283</v>
+        <v>-0.50654004562545207</v>
       </c>
       <c r="I1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.56369881531322519</v>
+        <v>0.73851635836701557</v>
       </c>
       <c r="J1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.74675455902202459</v>
+        <v>-0.77773151818274289</v>
       </c>
       <c r="K1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.17963733338466081</v>
+        <v>0.77793691973853307</v>
       </c>
       <c r="N1" t="s">
         <v>6</v>
@@ -3521,1451 +3517,1451 @@
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <f t="shared" ref="A2:K30" ca="1" si="1">2*RAND()-1</f>
-        <v>-0.31361476571013713</v>
+        <v>-0.17050331750400893</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.45492156163255593</v>
+        <v>-0.62320056870928719</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.92744278229979771</v>
+        <v>0.30778996330979136</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27060773672727567</v>
+        <v>0.44208137048849672</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31216225014250232</v>
+        <v>-9.7830281777177008E-2</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.7678446859186856E-2</v>
+        <v>-7.158479555960251E-2</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1368961145053369E-2</v>
+        <v>0.77052818127607714</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.27244714824013805</v>
+        <v>-0.30651912140884763</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94542702234451204</v>
+        <v>0.76883462546318038</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.41432929234355309</v>
+        <v>-0.97100766887311507</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87012599444792871</v>
+        <v>0.10586358146829244</v>
       </c>
       <c r="N2">
         <f ca="1">0.4*RAND() - 0.2</f>
-        <v>-1.203212186111155E-2</v>
+        <v>-0.14106997902336788</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.65881796049850383</v>
+        <v>0.28051218660085064</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.20585213174448236</v>
+        <v>-0.52489573747895424</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.40540414312357442</v>
+        <v>0.21587737813841623</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.5648900228467979</v>
+        <v>-0.28586431237073251</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44789117744665274</v>
+        <v>-0.89314418579672128</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25189481845559736</v>
+        <v>-0.68137531284758146</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.50927283812328428</v>
+        <v>-0.32949238559279781</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66202124470210522</v>
+        <v>-0.33904275595142574</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.49643396520200622</v>
+        <v>-0.43700187276815794</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.50488945269502539</v>
+        <v>-0.58541569570194185</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13473921366295261</v>
+        <v>-0.9648379511312406</v>
       </c>
       <c r="N3">
         <f t="shared" ref="N3:N30" ca="1" si="2">0.4*RAND() - 0.2</f>
-        <v>-1.6787647488696822E-2</v>
+        <v>-3.378175716077067E-2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89752350465248854</v>
+        <v>0.93364033900463594</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84827038162393142</v>
+        <v>-0.47874441739644524</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9633972415561356</v>
+        <v>0.21263206022609182</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17827263607082355</v>
+        <v>-0.18944582562943135</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.28011951932248014</v>
+        <v>-2.0739107937677526E-2</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.28106874760263501</v>
+        <v>-0.67975194318454624</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.3981156412513287</v>
+        <v>0.80104483142862049</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41549859408885692</v>
+        <v>-0.89523545924393999</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0121064576512637E-2</v>
+        <v>0.56211987337800129</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.35748054145167485</v>
+        <v>0.85147846163746954</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68366588199170897</v>
+        <v>-0.22078105471522891</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="2"/>
-        <v>-8.951540068066699E-3</v>
+        <v>4.3704992842835411E-3</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.38164516491839584</v>
+        <v>0.88713909433659444</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.1557296141399958E-2</v>
+        <v>-0.94793658655380097</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.93667313481381553</v>
+        <v>1.5476986462356734E-2</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.84425193639344176</v>
+        <v>-0.8765126541353776</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84689364472340167</v>
+        <v>0.13045587490542521</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3744905149225595E-3</v>
+        <v>0.16378444589064767</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.70153707828169254</v>
+        <v>-0.56184031659392319</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.63856667608590012</v>
+        <v>0.18194234240374119</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.72411424352029474</v>
+        <v>8.1253482322937609E-2</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.10607256670695331</v>
+        <v>0.30620726797496522</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2930241956686177</v>
+        <v>-3.3519507678666072E-2</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.17222241530858318</v>
+        <v>-0.11443606792118946</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56644534734050955</v>
+        <v>0.64340710906082488</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.14571831526989265</v>
+        <v>-0.12518474381795031</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41401483438476161</v>
+        <v>0.68063541512395487</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38677089016805843</v>
+        <v>-6.8075653696180183E-3</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96425437539186842</v>
+        <v>0.95106863980038248</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.438536202505313</v>
+        <v>0.46461928122813267</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.27892941410268501</v>
+        <v>9.8714555505083901E-2</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4269920435984087</v>
+        <v>0.56437558625898165</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5004088916977825E-3</v>
+        <v>-0.77248596905569089</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.97121668776707848</v>
+        <v>0.78985916449617011</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18391627397868993</v>
+        <v>-0.24598569354621014</v>
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="2"/>
-        <v>-3.5425965012064825E-2</v>
+        <v>-8.2417743501324345E-2</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.84624968312557236</v>
+        <v>0.26905161682402223</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.27276982977269326</v>
+        <v>-0.5514954787524271</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57358863569454943</v>
+        <v>-0.2148555682770994</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37252657592851079</v>
+        <v>-0.92860133363506758</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.77049987857446389</v>
+        <v>-0.40485907387300646</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.14069482940221079</v>
+        <v>-0.32140082259877167</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.81354555230436865</v>
+        <v>0.49805023015034977</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78556972510895196</v>
+        <v>-0.72590079346045822</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82611701195345555</v>
+        <v>-0.76047089781192367</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18616791402869426</v>
+        <v>-0.32783067405305322</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.0717301369316283E-2</v>
+        <v>-0.69484129363946789</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="2"/>
-        <v>-8.664832862554267E-2</v>
+        <v>1.9371428195445628E-2</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69437534680465962</v>
+        <v>-0.97898738202372471</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32216293828919462</v>
+        <v>-0.49000340075369309</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.80900635643115448</v>
+        <v>-0.43268325410778496</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.0207554580808971E-3</v>
+        <v>-0.40454542094273727</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.26525709121116403</v>
+        <v>0.9019041749976211</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.55877695283949746</v>
+        <v>-0.67282297988539397</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.76935078493925446</v>
+        <v>0.81544967498387511</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.92085888900487567</v>
+        <v>0.94245455837989445</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.88632607875382186</v>
+        <v>-0.31206617369219081</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66209263668177032</v>
+        <v>-0.5577676775410676</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.57663728344588194</v>
+        <v>-0.71590570460615877</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="2"/>
-        <v>9.8469001114026011E-3</v>
+        <v>0.16562924836125825</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.12038177045245657</v>
+        <v>-0.96824038891189823</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.36012823162524632</v>
+        <v>0.70611124970466488</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84965429019704608</v>
+        <v>-0.93576130982932693</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.79254520223820935</v>
+        <v>-0.69328253567116627</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70347150534231084</v>
+        <v>-0.96536398545734392</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.60565912021862145</v>
+        <v>0.28924742067493714</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.75976903488080683</v>
+        <v>-0.8259892369424644</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11889879097631506</v>
+        <v>0.99190458589347164</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.44406229299292566</v>
+        <v>0.9007266460920349</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15526149526494426</v>
+        <v>-0.50949328368031166</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.33016738469965556</v>
+        <v>-0.64573001155188892</v>
       </c>
       <c r="N9">
         <f t="shared" ca="1" si="2"/>
-        <v>0.12413056214160795</v>
+        <v>0.13168481477901872</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.23906480380244299</v>
+        <v>0.55327733088281716</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.63701974565596919</v>
+        <v>0.76991227730409006</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9798091699109337</v>
+        <v>-0.28942334922876034</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.87558449729290277</v>
+        <v>-0.32241228567706126</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30989859600995384</v>
+        <v>0.71597380881051143</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.60373565268555973</v>
+        <v>0.87054605688230691</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.71257502622494995</v>
+        <v>0.91404671520783509</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88013794513855026</v>
+        <v>-0.45271251670379042</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8055509988878462</v>
+        <v>-0.11179388690467951</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1286385705948199E-2</v>
+        <v>9.1702252368687454E-2</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23439100788220424</v>
+        <v>-0.50357923092538392</v>
       </c>
       <c r="N10">
         <f t="shared" ca="1" si="2"/>
-        <v>-6.3932817468782405E-2</v>
+        <v>-0.10120721917979797</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.55531310639384057</v>
+        <v>-0.42441181795449201</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.9257156757588776E-2</v>
+        <v>0.11071051741562465</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79032029234124668</v>
+        <v>-6.4001048930894866E-2</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.11434852058149203</v>
+        <v>0.20740944520345783</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.14247139313875823</v>
+        <v>0.34759410246502043</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64103757245008142</v>
+        <v>0.46857431670968519</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11010456956829251</v>
+        <v>0.61091146546928687</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38829599636655798</v>
+        <v>0.14105961673027911</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74033995115098805</v>
+        <v>0.34629562569407768</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.1865072442150606</v>
+        <v>-0.13738089046197</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.29666243778766055</v>
+        <v>-0.93226017211778833</v>
       </c>
       <c r="N11">
         <f t="shared" ca="1" si="2"/>
-        <v>-7.3023052783801001E-2</v>
+        <v>4.3129589683679997E-2</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5260078022690147E-2</v>
+        <v>-9.4438072078997681E-2</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.74570407176534781</v>
+        <v>-0.17920937167919337</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85843945764354057</v>
+        <v>0.37620209200194821</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28197470768813404</v>
+        <v>0.44483954949721394</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25569860658949528</v>
+        <v>-0.19583719315031489</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91841256981738528</v>
+        <v>-0.55865190414975419</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.72279236060004082</v>
+        <v>0.14751498104162919</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79718243930594679</v>
+        <v>0.17552242630952275</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7109682249835556E-2</v>
+        <v>-0.34710207592695674</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.58636305244568865</v>
+        <v>-4.0919375671344405E-3</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.417474964385248</v>
+        <v>-0.8663322817931054</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="2"/>
-        <v>2.121885668888418E-2</v>
+        <v>-2.9885181081866025E-2</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46555328449980515</v>
+        <v>-0.63956406226282603</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54640909044881436</v>
+        <v>6.0124402949708333E-2</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18594661115586431</v>
+        <v>-0.73814116064672564</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89936615503037864</v>
+        <v>-0.2960146617254531</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.65207530869873898</v>
+        <v>0.16494851249791442</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68818615985806497</v>
+        <v>-0.84769286673021305</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.60468845796712278</v>
+        <v>1.6583063965538214E-2</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79556622364574348</v>
+        <v>-0.74510744998795397</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.52177307227131764</v>
+        <v>-0.25601362145790008</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18641687722324041</v>
+        <v>-0.94193606606753399</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.96734193421915782</v>
+        <v>0.54470853563047128</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="2"/>
-        <v>0.10446311680898707</v>
+        <v>-1.4221212618066914E-2</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8790648319021228E-2</v>
+        <v>0.83617561781239891</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.51103592635065387</v>
+        <v>0.33673343194681649</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59034986365473618</v>
+        <v>0.43934130387445713</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.58258667876633563</v>
+        <v>9.1674059173812328E-2</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.20638484162338022</v>
+        <v>-0.53475983505607805</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74830397672263604</v>
+        <v>0.45880761811100768</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.78060722739129429</v>
+        <v>0.46477501274065336</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.99658550578105687</v>
+        <v>4.191219848690042E-2</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86412360941892263</v>
+        <v>-7.4178559487974693E-2</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.50468985696215296</v>
+        <v>0.60816408350181717</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66288474697556077</v>
+        <v>-0.78983828375739629</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="2"/>
-        <v>0.11013875457394628</v>
+        <v>0.11073803922843101</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.73363679865439324</v>
+        <v>-0.74406724145779268</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29095729605621923</v>
+        <v>-0.81476214154363369</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.92274959903331144</v>
+        <v>0.87903573801167911</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40715741042559683</v>
+        <v>-0.99546946051430774</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.4871686399557955E-2</v>
+        <v>-0.64838297993600058</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.87781860309594251</v>
+        <v>0.6053561075622107</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.92675832096483335</v>
+        <v>0.63992644582204616</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.74423450326238094</v>
+        <v>0.39250118564391201</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.40871455573586934</v>
+        <v>0.18686452649683472</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3227887227306194E-3</v>
+        <v>0.12188074914197533</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17636482073782123</v>
+        <v>-0.77344003542369255</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="2"/>
-        <v>-1.4248966070794122E-2</v>
+        <v>-0.15809618354584237</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.26354849897486776</v>
+        <v>0.42406960815434891</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.17684025558697636</v>
+        <v>0.19234215406797639</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.80700271090845344</v>
+        <v>-0.1864008616163344</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41305907411926412</v>
+        <v>0.68164913405868321</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.63885925610656424</v>
+        <v>0.59222808369069391</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39086733845179777</v>
+        <v>0.25585503232360773</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.76719638764731535</v>
+        <v>-0.1385362759947002</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.79988476100565253</v>
+        <v>0.80279168671269474</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.7025210754926563</v>
+        <v>0.24887635022448773</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11708818044606351</v>
+        <v>0.470071506038515</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10911298688924154</v>
+        <v>1.993588460506901E-2</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.15147092581456498</v>
+        <v>0.11298037652155613</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.49537120013704961</v>
+        <v>-0.78153736675294394</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.97404049635584711</v>
+        <v>0.54758501678634985</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.87301710002986077</v>
+        <v>0.91332565819218403</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72928449584633803</v>
+        <v>-0.10955269785669075</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.79695107005194843</v>
+        <v>0.27927187198669245</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.80612022879345369</v>
+        <v>0.66148811463375101</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.31007982702967363</v>
+        <v>-0.51657207216715628</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.10170654761379172</v>
+        <v>0.89948008511562305</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.46948473633512933</v>
+        <v>-0.17815378716193608</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5843014714932746</v>
+        <v>-0.50246557652108925</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.8145461565995316E-2</v>
+        <v>-0.45820283249143046</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="2"/>
-        <v>1.4922533602373111E-2</v>
+        <v>-0.18407407063141423</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.15295753043565785</v>
+        <v>-0.52121196552914251</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.65463357691494473</v>
+        <v>7.1298286521803034E-2</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.73832421612149401</v>
+        <v>0.22851982563347328</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.63746196562526292</v>
+        <v>0.62932316402150779</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.92886922030868502</v>
+        <v>0.59725653502915144</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53826539376781946</v>
+        <v>-0.97291669628593991</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.20601910865241679</v>
+        <v>0.97431505423825904</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.63650582944610679</v>
+        <v>0.75755622615754548</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.77023577787159159</v>
+        <v>0.94256641461462753</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.70745152952997237</v>
+        <v>-0.29761340133156966</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.14791696956217515</v>
+        <v>-0.81936653742352217</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="2"/>
-        <v>3.9332893918722633E-4</v>
+        <v>0.10687152853803988</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.3038805439705925E-2</v>
+        <v>-0.94203858489596337</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92644386345183527</v>
+        <v>0.32427143563645289</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.73191574587062491</v>
+        <v>0.92559843413292109</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.37676292602370287</v>
+        <v>0.9200128990677634</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.6124553040869356</v>
+        <v>-0.75107908056100459</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.87860352337362135</v>
+        <v>0.70671372765626561</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.57620776904736859</v>
+        <v>-0.63256158359561909</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.51609924064780133</v>
+        <v>-0.89445333762591916</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92006582576713147</v>
+        <v>-0.98465049219232736</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.14156141813674772</v>
+        <v>-0.53609610131197427</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.38846763223791481</v>
+        <v>0.40716805120086863</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.15996239871434162</v>
+        <v>9.7557980555484147E-2</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.14624983678289083</v>
+        <v>0.92761664474380501</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.47126908547791313</v>
+        <v>0.63954165443304034</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.9635551799174014E-2</v>
+        <v>-6.4360304527385059E-2</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.083602937320463E-2</v>
+        <v>0.61533468818986758</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.8270677901714738</v>
+        <v>-0.28156510441035643</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5528741896565601</v>
+        <v>-9.1953433903723125E-2</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67831481857346376</v>
+        <v>-0.52465970146924068</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.74992801168172996</v>
+        <v>0.16336017285130566</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.36192294030619587</v>
+        <v>-0.7656276368496735</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.57755020757079634</v>
+        <v>-0.53567701382847455</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.48063331980938395</v>
+        <v>-0.46007231109464564</v>
       </c>
       <c r="N20">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.19862519089775266</v>
+        <v>0.12659854997911901</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.37066099724532298</v>
+        <v>0.98493525627011436</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.87539482602283658</v>
+        <v>0.65383271017557942</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.83066307998466105</v>
+        <v>5.6418586776432633E-2</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.90366954889952678</v>
+        <v>0.31503598194597582</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.52641363779367789</v>
+        <v>0.67434994831017692</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.4245298931453747</v>
+        <v>7.1962634468964115E-2</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.14599877818441476</v>
+        <v>-0.32228432957438269</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.49627743389889067</v>
+        <v>-0.66152882210563657</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.68390566901061756</v>
+        <v>0.43824552557491825</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.71162195799161543</v>
+        <v>-0.488620268982775</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.45248151721555185</v>
+        <v>-0.70571761446431114</v>
       </c>
       <c r="N21">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.18998641573692523</v>
+        <v>0.12574059313884917</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.74691732049041804</v>
+        <v>-0.43255791535004628</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.48164291017125849</v>
+        <v>7.5473898339656342E-2</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3753738481590787</v>
+        <v>0.6262261813977763</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94405424469161847</v>
+        <v>0.8839879972035074</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39361313361842587</v>
+        <v>-0.86205575083772445</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16215523654369091</v>
+        <v>0.22155752903344506</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.71283278147936047</v>
+        <v>-0.14832258127452835</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.30401588432392956</v>
+        <v>-8.4076250080858728E-2</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.95064111302616272</v>
+        <v>-0.44615849664639895</v>
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.63574394968801418</v>
+        <v>0.27146348982107327</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0367276821375189E-2</v>
+        <v>-1.3255798926461448E-2</v>
       </c>
       <c r="N22">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.10269202910544256</v>
+        <v>0.16130549480518963</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.57435732417564789</v>
+        <v>0.73587606065320887</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>7.575658668836982E-2</v>
+        <v>0.10775197504980016</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.56790908584925681</v>
+        <v>-0.25441442357737554</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24557199706618138</v>
+        <v>0.16406001008307669</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35280545397595064</v>
+        <v>-0.9508034060998718</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.5049976469141653E-2</v>
+        <v>0.15025321639511002</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.83346204478505204</v>
+        <v>-0.73703286076500807</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.39567137266484398</v>
+        <v>0.10108612497152891</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0031691531205578E-2</v>
+        <v>0.17227701353588909</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.54429764140327785</v>
+        <v>-0.42740313103784522</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.77468661244372439</v>
+        <v>0.33491933585655609</v>
       </c>
       <c r="N23">
         <f t="shared" ca="1" si="2"/>
-        <v>-3.7465147799003062E-2</v>
+        <v>-6.1492384066372863E-2</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.19475874099101964</v>
+        <v>-0.90626198412948678</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.489190355787235E-2</v>
+        <v>-0.15713608876524532</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.97325660088133881</v>
+        <v>-0.81189352698321349</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22654113292139444</v>
+        <v>-0.80590652646346217</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69629082386688812</v>
+        <v>-7.9789093167811131E-2</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.99255071117280558</v>
+        <v>-0.70460856285495055</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.31361417949706816</v>
+        <v>0.95886102277674778</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92178031030014718</v>
+        <v>-0.9173880525456144</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.52755303104720808</v>
+        <v>0.27519891542443409</v>
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.44913206321734611</v>
+        <v>-0.64718095215581362</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.4543452818200056E-2</v>
+        <v>0.91781257033906716</v>
       </c>
       <c r="N24">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.13498434994140773</v>
+        <v>1.1719258525133197E-2</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72276612600455814</v>
+        <v>-0.20594822632226428</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26793183623596528</v>
+        <v>-0.14356639131942495</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60420137116000761</v>
+        <v>-9.5348134575590215E-4</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.57383058580576307</v>
+        <v>0.42636637219024864</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7218904027947355E-2</v>
+        <v>0.74992538776704309</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93233722920279227</v>
+        <v>-9.8915601974409739E-2</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.22224279125762925</v>
+        <v>0.50254794193880348</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.96792465982824449</v>
+        <v>-0.19224760100696447</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.87653586025496755</v>
+        <v>0.42199366560616047</v>
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.81607122370883078</v>
+        <v>-0.54655538863023834</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.86317239537794488</v>
+        <v>-0.39455149600332162</v>
       </c>
       <c r="N25">
         <f t="shared" ca="1" si="2"/>
-        <v>5.2358040923442095E-2</v>
+        <v>2.1418502477677348E-2</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.3850762184218794E-2</v>
+        <v>-0.45001972284126768</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.95070329724138092</v>
+        <v>-0.42942976193512639</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58337470433460381</v>
+        <v>0.50952345212713435</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.67918762364045127</v>
+        <v>-0.20857810734842253</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10834511598195196</v>
+        <v>0.223852369990164</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.31073974705142682</v>
+        <v>0.83910304961719095</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.97716704302748814</v>
+        <v>0.57709222608226352</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.15951682242617027</v>
+        <v>0.39156823398675056</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.17278988445272114</v>
+        <v>-0.3496324538153035</v>
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.962439899213134</v>
+        <v>0.69686564305322718</v>
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28522929340036196</v>
+        <v>-0.8665411608283291</v>
       </c>
       <c r="N26">
         <f t="shared" ca="1" si="2"/>
-        <v>-1.9125830493049445E-2</v>
+        <v>3.729282779219098E-2</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7004128266462406</v>
+        <v>-0.7603168726624594</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.2975611355480918E-2</v>
+        <v>-0.1401681612084329</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.55250912920827511</v>
+        <v>-1.7242331229443852E-2</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.91696981657017451</v>
+        <v>-0.10266291730998689</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10933422922528013</v>
+        <v>0.33740818909820303</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.20566347660819462</v>
+        <v>0.93261384947636206</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28820516017615083</v>
+        <v>0.99759009233783469</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.9646978649574987E-2</v>
+        <v>0.6649215110403488</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.57638532948283783</v>
+        <v>2.8995976208989305E-2</v>
       </c>
       <c r="J27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72889092679889278</v>
+        <v>-0.64713198193881949</v>
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.86327589351863065</v>
+        <v>-6.5003143967956145E-2</v>
       </c>
       <c r="N27">
         <f t="shared" ca="1" si="2"/>
-        <v>0.10386631467714857</v>
+        <v>-0.12778231308362914</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.71494262621715543</v>
+        <v>-2.3208893077420578E-2</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.16513696997953664</v>
+        <v>-0.22388892983959452</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.98281503117794822</v>
+        <v>-1.3256209474491243E-2</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.31993704446549809</v>
+        <v>0.64190044382947531</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.61648177273334626</v>
+        <v>0.62690120284444406</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="1"/>
-        <v>3.7576018924351917E-2</v>
+        <v>0.63691979744404459</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.19984457841075454</v>
+        <v>-0.93596804478868423</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.83055373231997942</v>
+        <v>0.81532013721355989</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.63835957027007373</v>
+        <v>-0.27288112308296908</v>
       </c>
       <c r="J28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59984133231734971</v>
+        <v>-0.46777472711579104</v>
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.17958479991446086</v>
+        <v>0.98891176712959217</v>
       </c>
       <c r="N28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.1498105953970208</v>
+        <v>-1.0304837635786018E-2</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" ca="1" si="1"/>
-        <v>9.8233031179056463E-2</v>
+        <v>-0.43893905610446682</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62714366396683174</v>
+        <v>3.3200016894605389E-2</v>
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35150241160631412</v>
+        <v>-0.32804099809583209</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.368224248268753</v>
+        <v>0.64294939774889892</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.70868708963228855</v>
+        <v>-0.12682594692022087</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7547362331262777E-2</v>
+        <v>-0.20628272750279297</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89857443109966839</v>
+        <v>0.359570366289923</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.52728036941351863</v>
+        <v>0.95659726097257702</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35799945008405021</v>
+        <v>7.7158906620271583E-3</v>
       </c>
       <c r="J29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12887860952226271</v>
+        <v>0.68968422604919022</v>
       </c>
       <c r="K29">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.12364935051682502</v>
+        <v>0.3692814489584233</v>
       </c>
       <c r="N29">
         <f t="shared" ca="1" si="2"/>
-        <v>8.9270644716957004E-2</v>
+        <v>4.35538949968301E-2</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" ca="1" si="1"/>
-        <v>5.2669103511228332E-2</v>
+        <v>0.36905633165051444</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.77658206648604411</v>
+        <v>0.68965673850623732</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.13012378532260827</v>
+        <v>0.39660537163151455</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26777791201951473</v>
+        <v>4.9369622028932802E-2</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.20706762962087377</v>
+        <v>-9.4942696986258346E-2</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.50418463753057607</v>
+        <v>0.89548809481938108</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.21819644173642394</v>
+        <v>0.73627414170189232</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.9733190697523455</v>
+        <v>-0.32640030628685501</v>
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59457674399413007</v>
+        <v>0.47749208127709242</v>
       </c>
       <c r="J30">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.60897897137131562</v>
+        <v>0.54641322933456093</v>
       </c>
       <c r="K30">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.33138558397368212</v>
+        <v>-0.47028486171852357</v>
       </c>
       <c r="N30">
         <f t="shared" ca="1" si="2"/>
-        <v>0.11066473236767643</v>
+        <v>-5.6644866995632648E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>